<commit_message>
feat(exchange): muda o tipo de leitura do arquivo de JSON para XLSX
</commit_message>
<xml_diff>
--- a/data/exchange.xlsx
+++ b/data/exchange.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C121"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,7 +452,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -460,12 +460,12 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>3.04322</v>
+        <v>1.75657</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -473,12 +473,12 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>3.514304761904762</v>
+        <v>1.759563636363636</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -486,12 +486,12 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3.871136363636363</v>
+        <v>1.693413043478261</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -499,12 +499,12 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>2.81645</v>
+        <v>1.841633333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -512,12 +512,12 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>2.634228571428571</v>
+        <v>1.77982</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -525,12 +525,12 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>3.223143478260869</v>
+        <v>1.769636363636364</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -538,12 +538,12 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>3.111738095238096</v>
+        <v>1.806528571428571</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -551,12 +551,12 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>3.061715</v>
+        <v>1.813190476190476</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -564,12 +564,12 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3.139477272727273</v>
+        <v>1.785843478260869</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -577,12 +577,12 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3.77646</v>
+        <v>1.71333</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -590,12 +590,12 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>3.880138095238095</v>
+        <v>1.6835</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -603,12 +603,12 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3.906457142857143</v>
+        <v>1.718709523809524</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -616,12 +616,12 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>3.565845</v>
+        <v>1.586447368421052</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -629,12 +629,12 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>3.209660869565217</v>
+        <v>1.597008695652174</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -642,12 +642,12 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>3.352268181818182</v>
+        <v>1.836886363636363</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -655,12 +655,12 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>3.973742105263157</v>
+        <v>1.66799</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -668,12 +668,12 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>4.05235</v>
+        <v>1.674914285714286</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -681,12 +681,12 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>3.275566666666667</v>
+        <v>1.563938095238095</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -694,12 +694,12 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>3.424477272727273</v>
+        <v>1.587042857142857</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -707,12 +707,12 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>3.539290476190476</v>
+        <v>1.613490909090909</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -720,12 +720,12 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>3.703918181818182</v>
+        <v>1.6591</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -733,12 +733,12 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>3.34203</v>
+        <v>1.79049</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -746,12 +746,12 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>3.185845</v>
+        <v>1.77257</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -759,12 +759,12 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>3.256371428571428</v>
+        <v>1.749776190476191</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -772,12 +772,12 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>3.136172222222222</v>
+        <v>1.854835</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -785,12 +785,12 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>3.150917391304348</v>
+        <v>2.02944347826087</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -798,12 +798,12 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>3.291915</v>
+        <v>2.077835</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -811,12 +811,12 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>3.104194444444444</v>
+        <v>1.718394736842106</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -824,12 +824,12 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>3.196609090909091</v>
+        <v>1.789681818181818</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -837,12 +837,12 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>3.206138095238095</v>
+        <v>2.028736363636364</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -850,12 +850,12 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>3.295366666666666</v>
+        <v>2.049195</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -863,12 +863,12 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>3.209509090909091</v>
+        <v>1.985990909090909</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -876,12 +876,12 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>3.127930434782609</v>
+        <v>1.795309090909091</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -889,12 +889,12 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>3.25938</v>
+        <v>2.06775</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -902,12 +902,12 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>3.191228571428571</v>
+        <v>2.029845454545455</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -915,12 +915,12 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>3.13479</v>
+        <v>2.028078947368421</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -928,12 +928,12 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3.407495238095238</v>
+        <v>2.002213636363636</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -941,12 +941,12 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>3.92975652173913</v>
+        <v>2.342190909090909</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -954,12 +954,12 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>3.885055</v>
+        <v>2.345485714285714</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -967,12 +967,12 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>3.2415</v>
+        <v>1.97325</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -980,12 +980,12 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>3.210609090909091</v>
+        <v>2.031077272727273</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -993,12 +993,12 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>3.828763636363636</v>
+        <v>2.252169565217391</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -1006,12 +1006,12 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>3.773171428571428</v>
+        <v>2.172955</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -1019,12 +1019,12 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>3.636057142857143</v>
+        <v>2.034842857142857</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -1032,12 +1032,12 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>3.279214285714286</v>
+        <v>1.98284</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -1045,12 +1045,12 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>3.786665</v>
+        <v>2.29535</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -1058,12 +1058,12 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>3.758409090909091</v>
+        <v>2.188647826086957</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -1071,12 +1071,12 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4.116547368421053</v>
+        <v>2.270509523809524</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -1084,12 +1084,12 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>3.896157142857143</v>
+        <v>2.23277</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -1097,12 +1097,12 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>4.019981818181818</v>
+        <v>2.268028571428571</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -1110,12 +1110,12 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>4.109590476190476</v>
+        <v>2.639363636363636</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -1123,12 +1123,12 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>3.723625</v>
+        <v>2.38368</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -1136,12 +1136,12 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>3.741681818181819</v>
+        <v>2.382209090909091</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -1149,12 +1149,12 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.779339130434783</v>
+        <v>2.224647826086957</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -1162,12 +1162,12 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3.858826315789474</v>
+        <v>2.23547</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -1175,12 +1175,12 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4.001518181818182</v>
+        <v>2.220880952380953</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -1188,12 +1188,12 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3.846484210526316</v>
+        <v>2.326089473684211</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -1201,12 +1201,12 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>4.155345</v>
+        <v>2.548365</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -1214,12 +1214,12 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>4.086986956521739</v>
+        <v>2.448260869565217</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -1227,12 +1227,12 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>4.1215</v>
+        <v>2.332868181818182</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -1240,12 +1240,12 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>5.32558</v>
+        <v>3.04322</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B63" t="inlineStr">
         <is>
@@ -1253,12 +1253,12 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>5.461233333333333</v>
+        <v>3.514304761904762</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B64" t="inlineStr">
         <is>
@@ -1266,12 +1266,12 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>5.145586363636363</v>
+        <v>3.871136363636363</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B65" t="inlineStr">
         <is>
@@ -1279,12 +1279,12 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>4.341011111111111</v>
+        <v>2.81645</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B66" t="inlineStr">
         <is>
@@ -1292,12 +1292,12 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>4.149463636363636</v>
+        <v>2.634228571428571</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B67" t="inlineStr">
         <is>
@@ -1305,12 +1305,12 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>5.280191304347826</v>
+        <v>3.223143478260869</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B68" t="inlineStr">
         <is>
@@ -1318,12 +1318,12 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>5.1966</v>
+        <v>3.111738095238096</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B69" t="inlineStr">
         <is>
@@ -1331,12 +1331,12 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>5.643445</v>
+        <v>3.061715</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B70" t="inlineStr">
         <is>
@@ -1344,12 +1344,12 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>4.883854545454546</v>
+        <v>3.139477272727273</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B71" t="inlineStr">
         <is>
@@ -1357,12 +1357,12 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>5.417835</v>
+        <v>3.77646</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B72" t="inlineStr">
         <is>
@@ -1370,12 +1370,12 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>5.625790476190476</v>
+        <v>3.880138095238095</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="B73" t="inlineStr">
         <is>
@@ -1383,12 +1383,12 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>5.399485714285714</v>
+        <v>3.906457142857143</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B74" t="inlineStr">
         <is>
@@ -1396,12 +1396,12 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>5.562135</v>
+        <v>3.565845</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B75" t="inlineStr">
         <is>
@@ -1409,12 +1409,12 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>5.251718181818182</v>
+        <v>3.209660869565217</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
@@ -1422,12 +1422,12 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>5.651391304347826</v>
+        <v>3.352268181818182</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
@@ -1435,12 +1435,12 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>5.416494444444444</v>
+        <v>3.973742105263157</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B78" t="inlineStr">
         <is>
@@ -1448,12 +1448,12 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>5.356244999999999</v>
+        <v>4.05235</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
@@ -1461,12 +1461,12 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>5.156704545454546</v>
+        <v>3.275566666666667</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
@@ -1474,12 +1474,12 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>5.031904761904762</v>
+        <v>3.424477272727273</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
@@ -1487,12 +1487,12 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>5.291057142857143</v>
+        <v>3.539290476190476</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B82" t="inlineStr">
         <is>
@@ -1500,12 +1500,12 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>5.646147826086957</v>
+        <v>3.703918181818182</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
@@ -1513,12 +1513,12 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>5.556859999999999</v>
+        <v>3.34203</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B84" t="inlineStr">
         <is>
@@ -1526,12 +1526,12 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>5.53998</v>
+        <v>3.185845</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
@@ -1539,12 +1539,12 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>5.279690476190477</v>
+        <v>3.256371428571428</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B86" t="inlineStr">
         <is>
@@ -1552,12 +1552,12 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>4.758015789473684</v>
+        <v>3.136172222222222</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
@@ -1565,12 +1565,12 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>5.143286956521739</v>
+        <v>3.150917391304348</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B88" t="inlineStr">
         <is>
@@ -1578,12 +1578,12 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>5.242431818181818</v>
+        <v>3.291915</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
@@ -1591,12 +1591,12 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>5.196578947368421</v>
+        <v>3.104194444444444</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B90" t="inlineStr">
         <is>
@@ -1604,12 +1604,12 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>5.534104761904762</v>
+        <v>3.196609090909091</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
@@ -1617,12 +1617,12 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5.368071428571429</v>
+        <v>3.206138095238095</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
@@ -1630,12 +1630,12 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>5.049209523809524</v>
+        <v>3.295366666666666</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B93" t="inlineStr">
         <is>
@@ -1643,12 +1643,12 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>4.95505</v>
+        <v>3.209509090909091</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
@@ -1656,12 +1656,12 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>4.968381818181818</v>
+        <v>3.127930434782609</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B95" t="inlineStr">
         <is>
@@ -1669,12 +1669,12 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>5.274649999999999</v>
+        <v>3.25938</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
@@ -1682,12 +1682,12 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>5.2503</v>
+        <v>3.191228571428571</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="B97" t="inlineStr">
         <is>
@@ -1695,12 +1695,12 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>5.236957142857143</v>
+        <v>3.13479</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
@@ -1708,12 +1708,12 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>5.019733333333333</v>
+        <v>3.407495238095238</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
@@ -1721,12 +1721,12 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>4.903543478260869</v>
+        <v>3.92975652173913</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B100" t="inlineStr">
         <is>
@@ -1734,12 +1734,12 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>4.897245</v>
+        <v>3.885055</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
@@ -1747,12 +1747,12 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>5.171688888888889</v>
+        <v>3.2415</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B102" t="inlineStr">
         <is>
@@ -1760,12 +1760,12 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>5.200681818181819</v>
+        <v>3.210609090909091</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
@@ -1773,12 +1773,12 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>4.800833333333333</v>
+        <v>3.828763636363636</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B104" t="inlineStr">
         <is>
@@ -1786,12 +1786,12 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>4.851566666666667</v>
+        <v>3.773171428571428</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
@@ -1799,12 +1799,12 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>4.982836363636364</v>
+        <v>3.636057142857143</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B106" t="inlineStr">
         <is>
@@ -1812,12 +1812,12 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>5.211460869565218</v>
+        <v>3.279214285714286</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
@@ -1825,12 +1825,12 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>4.89834</v>
+        <v>3.786665</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B108" t="inlineStr">
         <is>
@@ -1838,12 +1838,12 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>5.064842857142857</v>
+        <v>3.758409090909091</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
@@ -1851,12 +1851,12 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>4.93699</v>
+        <v>4.116547368421053</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B110" t="inlineStr">
         <is>
@@ -1864,12 +1864,12 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>5.129095454545455</v>
+        <v>3.896157142857143</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
@@ -1877,12 +1877,12 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>5.552613636363636</v>
+        <v>4.019981818181818</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
@@ -1890,12 +1890,12 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>6.097028571428571</v>
+        <v>4.109590476190476</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B113" t="inlineStr">
         <is>
@@ -1903,12 +1903,12 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>4.964389473684211</v>
+        <v>3.723625</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
@@ -1916,12 +1916,12 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>4.914395454545454</v>
+        <v>3.741681818181819</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B115" t="inlineStr">
         <is>
@@ -1929,12 +1929,12 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>5.542047826086956</v>
+        <v>3.779339130434783</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
@@ -1942,12 +1942,12 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>5.388975</v>
+        <v>3.858826315789474</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B117" t="inlineStr">
         <is>
@@ -1955,12 +1955,12 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>5.133047619047619</v>
+        <v>4.001518181818182</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
@@ -1968,12 +1968,12 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>4.980135</v>
+        <v>3.846484210526316</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B119" t="inlineStr">
         <is>
@@ -1981,12 +1981,12 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>5.807057894736842</v>
+        <v>4.155345</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
@@ -1994,19 +1994,799 @@
         </is>
       </c>
       <c r="C120" t="n">
-        <v>5.624108695652174</v>
+        <v>4.086986956521739</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
+        <v>2019</v>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="C121" t="n">
+        <v>4.1215</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="C122" t="n">
+        <v>5.32558</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="C123" t="n">
+        <v>5.461233333333333</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>Dezembro</t>
+        </is>
+      </c>
+      <c r="C124" t="n">
+        <v>5.145586363636363</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="C125" t="n">
+        <v>4.341011111111111</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="C126" t="n">
+        <v>4.149463636363636</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="C127" t="n">
+        <v>5.280191304347826</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="C128" t="n">
+        <v>5.1966</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C129" t="n">
+        <v>5.643445</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="C130" t="n">
+        <v>4.883854545454546</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>Novembro</t>
+        </is>
+      </c>
+      <c r="C131" t="n">
+        <v>5.417835</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C132" t="n">
+        <v>5.625790476190476</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="C133" t="n">
+        <v>5.399485714285714</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="C134" t="n">
+        <v>5.562135</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="C135" t="n">
+        <v>5.251718181818182</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>Dezembro</t>
+        </is>
+      </c>
+      <c r="C136" t="n">
+        <v>5.651391304347826</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="C137" t="n">
+        <v>5.416494444444444</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="C138" t="n">
+        <v>5.356244999999999</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="C139" t="n">
+        <v>5.156704545454546</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>5.031904761904762</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>5.291057142857143</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>5.646147826086957</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>Novembro</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>5.556859999999999</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>5.53998</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>5.279690476190477</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>4.758015789473684</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>5.143286956521739</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>Dezembro</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>5.242431818181818</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="C149" t="n">
+        <v>5.196578947368421</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="C150" t="n">
+        <v>5.534104761904762</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="C151" t="n">
+        <v>5.368071428571429</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="C152" t="n">
+        <v>5.049209523809524</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C153" t="n">
+        <v>4.95505</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="C154" t="n">
+        <v>4.968381818181818</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>Novembro</t>
+        </is>
+      </c>
+      <c r="C155" t="n">
+        <v>5.274649999999999</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C156" t="n">
+        <v>5.2503</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="C157" t="n">
+        <v>5.236957142857143</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="C158" t="n">
+        <v>5.019733333333333</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="C159" t="n">
+        <v>4.903543478260869</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Dezembro</t>
+        </is>
+      </c>
+      <c r="C160" t="n">
+        <v>4.897245</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="C161" t="n">
+        <v>5.171688888888889</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="C162" t="n">
+        <v>5.200681818181819</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="C163" t="n">
+        <v>4.800833333333333</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="C164" t="n">
+        <v>4.851566666666667</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C165" t="n">
+        <v>4.982836363636364</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="C166" t="n">
+        <v>5.211460869565218</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>Novembro</t>
+        </is>
+      </c>
+      <c r="C167" t="n">
+        <v>4.89834</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C168" t="n">
+        <v>5.064842857142857</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2023</v>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>Setembro</t>
+        </is>
+      </c>
+      <c r="C169" t="n">
+        <v>4.93699</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
         <v>2024</v>
       </c>
-      <c r="B121" t="inlineStr">
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Abril</t>
+        </is>
+      </c>
+      <c r="C170" t="n">
+        <v>5.129095454545455</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>Agosto</t>
+        </is>
+      </c>
+      <c r="C171" t="n">
+        <v>5.552613636363636</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>Dezembro</t>
+        </is>
+      </c>
+      <c r="C172" t="n">
+        <v>6.097028571428571</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Fevereiro</t>
+        </is>
+      </c>
+      <c r="C173" t="n">
+        <v>4.964389473684211</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Janeiro</t>
+        </is>
+      </c>
+      <c r="C174" t="n">
+        <v>4.914395454545454</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Julho</t>
+        </is>
+      </c>
+      <c r="C175" t="n">
+        <v>5.542047826086956</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Junho</t>
+        </is>
+      </c>
+      <c r="C176" t="n">
+        <v>5.388975</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Maio</t>
+        </is>
+      </c>
+      <c r="C177" t="n">
+        <v>5.133047619047619</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>Março</t>
+        </is>
+      </c>
+      <c r="C178" t="n">
+        <v>4.980135</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>Novembro</t>
+        </is>
+      </c>
+      <c r="C179" t="n">
+        <v>5.807057894736842</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Outubro</t>
+        </is>
+      </c>
+      <c r="C180" t="n">
+        <v>5.624108695652174</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="n">
+        <v>2024</v>
+      </c>
+      <c r="B181" t="inlineStr">
         <is>
           <t>Setembro</t>
         </is>
       </c>
-      <c r="C121" t="n">
+      <c r="C181" t="n">
         <v>5.541566666666666</v>
       </c>
     </row>

</xml_diff>